<commit_message>
memperbarui excel data analisis, tambah readme, memperbarui EDA
</commit_message>
<xml_diff>
--- a/data-cleaned/sales.xlsx
+++ b/data-cleaned/sales.xlsx
@@ -17,8 +17,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>

</xml_diff>